<commit_message>
tambah kurang kali bagi
</commit_message>
<xml_diff>
--- a/supportfile/Copy of RPD Filling Rollie (3).xlsx
+++ b/supportfile/Copy of RPD Filling Rollie (3).xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="90" windowWidth="20115" windowHeight="9270" activeTab="2"/>
+    <workbookView xWindow="240" yWindow="90" windowWidth="20115" windowHeight="9270" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Rollie RPD Filling" sheetId="3" r:id="rId1"/>
@@ -1330,7 +1330,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="107">
+  <cellXfs count="108">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -1619,6 +1619,9 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -4924,11 +4927,11 @@
       <c r="D26" s="33" t="s">
         <v>222</v>
       </c>
-      <c r="E26" s="105" t="s">
+      <c r="E26" s="106" t="s">
         <v>219</v>
       </c>
-      <c r="F26" s="105"/>
-      <c r="G26" s="105"/>
+      <c r="F26" s="106"/>
+      <c r="G26" s="106"/>
     </row>
     <row r="27" spans="2:9" ht="21" customHeight="1">
       <c r="B27" s="48" t="s">
@@ -4940,9 +4943,9 @@
       <c r="D27" s="50" t="s">
         <v>271</v>
       </c>
-      <c r="E27" s="105"/>
-      <c r="F27" s="105"/>
-      <c r="G27" s="105"/>
+      <c r="E27" s="106"/>
+      <c r="F27" s="106"/>
+      <c r="G27" s="106"/>
       <c r="I27" t="s">
         <v>223</v>
       </c>
@@ -4957,9 +4960,9 @@
       <c r="D28" s="50" t="s">
         <v>56</v>
       </c>
-      <c r="E28" s="105"/>
-      <c r="F28" s="105"/>
-      <c r="G28" s="105"/>
+      <c r="E28" s="106"/>
+      <c r="F28" s="106"/>
+      <c r="G28" s="106"/>
     </row>
     <row r="29" spans="2:9" ht="21" customHeight="1">
       <c r="B29" s="48" t="s">
@@ -4971,9 +4974,9 @@
       <c r="D29" s="50" t="s">
         <v>45</v>
       </c>
-      <c r="E29" s="105"/>
-      <c r="F29" s="105"/>
-      <c r="G29" s="105"/>
+      <c r="E29" s="106"/>
+      <c r="F29" s="106"/>
+      <c r="G29" s="106"/>
     </row>
     <row r="30" spans="2:9" ht="21" customHeight="1">
       <c r="B30" s="48" t="s">
@@ -4985,9 +4988,9 @@
       <c r="D30" s="50" t="s">
         <v>58</v>
       </c>
-      <c r="E30" s="105"/>
-      <c r="F30" s="105"/>
-      <c r="G30" s="105"/>
+      <c r="E30" s="106"/>
+      <c r="F30" s="106"/>
+      <c r="G30" s="106"/>
     </row>
     <row r="31" spans="2:9" ht="21" customHeight="1"/>
     <row r="35" spans="2:4">
@@ -5089,7 +5092,7 @@
   <dimension ref="B3:L113"/>
   <sheetViews>
     <sheetView showGridLines="0" topLeftCell="A60" workbookViewId="0">
-      <selection activeCell="L29" sqref="L29"/>
+      <selection activeCell="D72" sqref="D72"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -5301,11 +5304,11 @@
       <c r="D26" s="33" t="s">
         <v>222</v>
       </c>
-      <c r="E26" s="105" t="s">
+      <c r="E26" s="106" t="s">
         <v>219</v>
       </c>
-      <c r="F26" s="105"/>
-      <c r="G26" s="105"/>
+      <c r="F26" s="106"/>
+      <c r="G26" s="106"/>
     </row>
     <row r="27" spans="2:9" ht="21" customHeight="1">
       <c r="B27" s="48" t="s">
@@ -5317,9 +5320,9 @@
       <c r="D27" s="50" t="s">
         <v>54</v>
       </c>
-      <c r="E27" s="105"/>
-      <c r="F27" s="105"/>
-      <c r="G27" s="105"/>
+      <c r="E27" s="106"/>
+      <c r="F27" s="106"/>
+      <c r="G27" s="106"/>
       <c r="I27" t="s">
         <v>223</v>
       </c>
@@ -5334,9 +5337,9 @@
       <c r="D28" s="50" t="s">
         <v>56</v>
       </c>
-      <c r="E28" s="105"/>
-      <c r="F28" s="105"/>
-      <c r="G28" s="105"/>
+      <c r="E28" s="106"/>
+      <c r="F28" s="106"/>
+      <c r="G28" s="106"/>
     </row>
     <row r="29" spans="2:9" ht="21" customHeight="1">
       <c r="B29" s="48" t="s">
@@ -5348,9 +5351,9 @@
       <c r="D29" s="50" t="s">
         <v>45</v>
       </c>
-      <c r="E29" s="105"/>
-      <c r="F29" s="105"/>
-      <c r="G29" s="105"/>
+      <c r="E29" s="106"/>
+      <c r="F29" s="106"/>
+      <c r="G29" s="106"/>
     </row>
     <row r="30" spans="2:9" ht="21" customHeight="1">
       <c r="B30" s="48" t="s">
@@ -5362,9 +5365,9 @@
       <c r="D30" s="50" t="s">
         <v>58</v>
       </c>
-      <c r="E30" s="105"/>
-      <c r="F30" s="105"/>
-      <c r="G30" s="105"/>
+      <c r="E30" s="106"/>
+      <c r="F30" s="106"/>
+      <c r="G30" s="106"/>
     </row>
     <row r="31" spans="2:9" ht="21" customHeight="1"/>
     <row r="34" spans="2:12" hidden="1"/>
@@ -5781,7 +5784,7 @@
         <v>21</v>
       </c>
       <c r="C72" s="34"/>
-      <c r="D72" s="50" t="s">
+      <c r="D72" s="105" t="s">
         <v>37</v>
       </c>
       <c r="E72" s="34"/>
@@ -6130,8 +6133,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A3:L108"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+    <sheetView showGridLines="0" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="G67" sqref="E26:G67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -6343,11 +6346,11 @@
       <c r="D26" s="33" t="s">
         <v>222</v>
       </c>
-      <c r="E26" s="105" t="s">
+      <c r="E26" s="106" t="s">
         <v>219</v>
       </c>
-      <c r="F26" s="105"/>
-      <c r="G26" s="105"/>
+      <c r="F26" s="106"/>
+      <c r="G26" s="106"/>
     </row>
     <row r="27" spans="2:9" ht="21" customHeight="1">
       <c r="B27" s="48" t="s">
@@ -6359,9 +6362,9 @@
       <c r="D27" s="50" t="s">
         <v>271</v>
       </c>
-      <c r="E27" s="105"/>
-      <c r="F27" s="105"/>
-      <c r="G27" s="105"/>
+      <c r="E27" s="106"/>
+      <c r="F27" s="106"/>
+      <c r="G27" s="106"/>
       <c r="I27" t="s">
         <v>223</v>
       </c>
@@ -6376,9 +6379,9 @@
       <c r="D28" s="50" t="s">
         <v>56</v>
       </c>
-      <c r="E28" s="105"/>
-      <c r="F28" s="105"/>
-      <c r="G28" s="105"/>
+      <c r="E28" s="106"/>
+      <c r="F28" s="106"/>
+      <c r="G28" s="106"/>
     </row>
     <row r="29" spans="2:9" ht="21" customHeight="1">
       <c r="B29" s="48" t="s">
@@ -6390,9 +6393,9 @@
       <c r="D29" s="50" t="s">
         <v>45</v>
       </c>
-      <c r="E29" s="105"/>
-      <c r="F29" s="105"/>
-      <c r="G29" s="105"/>
+      <c r="E29" s="106"/>
+      <c r="F29" s="106"/>
+      <c r="G29" s="106"/>
     </row>
     <row r="30" spans="2:9" ht="21" customHeight="1">
       <c r="B30" s="48" t="s">
@@ -6404,9 +6407,9 @@
       <c r="D30" s="50" t="s">
         <v>58</v>
       </c>
-      <c r="E30" s="105"/>
-      <c r="F30" s="105"/>
-      <c r="G30" s="105"/>
+      <c r="E30" s="106"/>
+      <c r="F30" s="106"/>
+      <c r="G30" s="106"/>
     </row>
     <row r="31" spans="2:9" ht="21" customHeight="1"/>
     <row r="34" spans="2:12" hidden="1"/>
@@ -7063,8 +7066,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AC246"/>
   <sheetViews>
-    <sheetView topLeftCell="F1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="U10" sqref="U10:U11"/>
+    <sheetView topLeftCell="E4" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="Y6" sqref="Y6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -20199,8 +20202,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AE42"/>
   <sheetViews>
-    <sheetView zoomScale="84" zoomScaleNormal="84" workbookViewId="0">
-      <selection activeCell="R5" sqref="R5"/>
+    <sheetView tabSelected="1" zoomScale="84" zoomScaleNormal="84" workbookViewId="0">
+      <selection activeCell="M5" sqref="M5:M6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -20331,27 +20334,27 @@
       <c r="AE3" s="61"/>
     </row>
     <row r="4" spans="1:31" ht="15.75" thickBot="1">
-      <c r="D4" s="106" t="s">
+      <c r="D4" s="107" t="s">
         <v>268</v>
       </c>
-      <c r="E4" s="106"/>
-      <c r="F4" s="106"/>
+      <c r="E4" s="107"/>
+      <c r="F4" s="107"/>
       <c r="I4" s="62" t="s">
         <v>265</v>
       </c>
       <c r="M4" s="62" t="s">
         <v>266</v>
       </c>
-      <c r="N4" s="106" t="s">
+      <c r="N4" s="107" t="s">
         <v>267</v>
       </c>
-      <c r="O4" s="106"/>
-      <c r="P4" s="106" t="s">
+      <c r="O4" s="107"/>
+      <c r="P4" s="107" t="s">
         <v>268</v>
       </c>
-      <c r="Q4" s="106"/>
-      <c r="R4" s="106"/>
-      <c r="S4" s="106"/>
+      <c r="Q4" s="107"/>
+      <c r="R4" s="107"/>
+      <c r="S4" s="107"/>
     </row>
     <row r="5" spans="1:31" ht="24.75" thickTop="1">
       <c r="A5" s="70" t="s">

</xml_diff>